<commit_message>
fix bug: exporting to an existed excel file will brake it.
</commit_message>
<xml_diff>
--- a/assets/excels/test.xlsx
+++ b/assets/excels/test.xlsx
@@ -3,56 +3,67 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\gg_project\GDScriptConfigTableTool\assets\excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5368E91-C06A-46B3-93AF-95EDC8813380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3108" yWindow="1524" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="4128" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="s1" sheetId="8" r:id="rId5"/>
+    <sheet name="s1" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">测试名1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">测试名2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">test_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>测试名1</t>
+  </si>
+  <si>
+    <t>test_name_1</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>测试名2</t>
+  </si>
+  <si>
+    <t>test_name_2</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>数组类型</t>
+  </si>
+  <si>
+    <t>test_name_3</t>
+  </si>
+  <si>
+    <t>test_name_4</t>
+  </si>
+  <si>
+    <t>Dictionary</t>
+  </si>
+  <si>
+    <t>bu</t>
+  </si>
+  <si>
+    <t>{"a": 1.4}</t>
     <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">test_name_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -91,69 +102,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFF"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,43 +127,8 @@
         <fgColor rgb="FF525252"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00E7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A9D08E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A9D08E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00525252"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00525252"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -234,77 +151,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+  </cellStyleXfs>
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -317,44 +173,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -363,11 +183,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -668,24 +488,21 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5625" style="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5625" style="14" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5625" style="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5625" style="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" width="21.5546875" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24" customHeight="1">
+    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -695,11 +512,11 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>6</v>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -709,11 +526,11 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" ht="14" customHeight="1">
+    <row r="3" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -721,33 +538,20 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="H13" t="s">
-        <v>8</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update ConfigTable_template to fit Godot4 GDScript2.0 Grammar Add support for relative path
</commit_message>
<xml_diff>
--- a/assets/excels/test.xlsx
+++ b/assets/excels/test.xlsx
@@ -3,67 +3,65 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\gg_project\GDScriptConfigTableTool\assets\excels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5368E91-C06A-46B3-93AF-95EDC8813380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4128" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4128" yWindow="1884" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
-    <sheet name="s1" sheetId="8" r:id="rId1"/>
+    <sheet name="s1" sheetId="12" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>测试名1</t>
-  </si>
-  <si>
-    <t>test_name_1</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>测试名2</t>
-  </si>
-  <si>
-    <t>test_name_2</t>
-  </si>
-  <si>
-    <t>Real</t>
-  </si>
-  <si>
-    <t>数组类型</t>
-  </si>
-  <si>
-    <t>test_name_3</t>
-  </si>
-  <si>
-    <t>test_name_4</t>
-  </si>
-  <si>
-    <t>Dictionary</t>
-  </si>
-  <si>
-    <t>bu</t>
-  </si>
-  <si>
-    <t>{"a": 1.4}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">测试名1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">测试名2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">数组类型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"a": 1.4}</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">bu666</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -104,8 +102,88 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +205,38 @@
         <fgColor rgb="FF525252"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00525252"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00525252"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -151,16 +259,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+  </cellStyleXfs>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -175,6 +344,54 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,11 +400,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,70 +705,71 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="21.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5625" style="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5625" style="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5625" style="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5625" style="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
+      <c r="D1" s="19" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>